<commit_message>
adding to failure log
</commit_message>
<xml_diff>
--- a/Part 3 - Failure Log.xlsx
+++ b/Part 3 - Failure Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Test #</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Create a post with 15 characters or less</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Reading rentFlag of the unit, exit rent() if rentFlag == "T"</t>
+  </si>
+  <si>
+    <t>Setting flag to check if user logged in, then reading that flag when login() called</t>
+  </si>
+  <si>
+    <t>Setting flag to check if rental already made in session, then checking that flag when post() called</t>
+  </si>
+  <si>
+    <t>Parsing user input as int, then warning user the max length of a rental is 14 days (if user input &gt; 14), and setting the numNights variable to 14.</t>
   </si>
 </sst>
 </file>
@@ -199,13 +214,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +526,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +603,12 @@
       <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -709,7 +731,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -720,7 +742,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -731,7 +753,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -742,7 +764,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -753,7 +775,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -764,7 +786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -775,7 +797,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -786,7 +808,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -797,7 +819,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -808,7 +830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -819,7 +841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -829,8 +851,14 @@
       <c r="C27" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -841,7 +869,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -852,7 +880,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -863,7 +891,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -874,7 +902,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -884,8 +912,14 @@
       <c r="C32" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -896,7 +930,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -906,8 +940,14 @@
       <c r="C34" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>

</xml_diff>